<commit_message>
Expanded allocate to move across all rows and columns
</commit_message>
<xml_diff>
--- a/staff.xlsx
+++ b/staff.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara.brumfield\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara.brumfield\Documents\_COVID-19\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
     <sheet name="min" sheetId="2" r:id="rId2"/>
+    <sheet name="diff" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>svc</t>
   </si>
@@ -414,7 +415,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,10 +845,13 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -891,6 +895,31 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>SUM(C2:I2)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -899,6 +928,16 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="0">SUM(C3:I3)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -907,6 +946,28 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>148</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -915,6 +976,31 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -923,6 +1009,13 @@
       <c r="B6">
         <v>3</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -931,6 +1024,22 @@
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -939,6 +1048,22 @@
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -947,6 +1072,13 @@
       <c r="B9">
         <v>3</v>
       </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -955,6 +1087,10 @@
       <c r="B10">
         <v>4</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -963,6 +1099,22 @@
       <c r="B11">
         <v>4</v>
       </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -971,6 +1123,13 @@
       <c r="B12">
         <v>4</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -978,6 +1137,549 @@
       </c>
       <c r="B13">
         <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>current!C2-min!C2</f>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>current!D2-min!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>current!E2-min!E2</f>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>current!F2-min!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>current!G2-min!G2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>current!H2-min!H2</f>
+        <v>-5</v>
+      </c>
+      <c r="I2">
+        <f>current!I2-min!I2</f>
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f>current!J2-min!J2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>current!C3-min!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>current!D3-min!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>current!E3-min!E3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>current!F3-min!F3</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>current!G3-min!G3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>current!H3-min!H3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>current!I3-min!I3</f>
+        <v>-2</v>
+      </c>
+      <c r="J3">
+        <f>current!J3-min!J3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>current!C4-min!C4</f>
+        <v>-26</v>
+      </c>
+      <c r="D4">
+        <f>current!D4-min!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>current!E4-min!E4</f>
+        <v>-4</v>
+      </c>
+      <c r="F4">
+        <f>current!F4-min!F4</f>
+        <v>-4</v>
+      </c>
+      <c r="G4">
+        <f>current!G4-min!G4</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>current!H4-min!H4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>current!I4-min!I4</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>current!J4-min!J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>current!C5-min!C5</f>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>current!D5-min!D5</f>
+        <v>-6</v>
+      </c>
+      <c r="E5">
+        <f>current!E5-min!E5</f>
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <f>current!F5-min!F5</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>current!G5-min!G5</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>current!H5-min!H5</f>
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f>current!I5-min!I5</f>
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <f>current!J5-min!J5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f>current!C6-min!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>current!D6-min!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>current!E6-min!E6</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>current!F6-min!F6</f>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <f>current!G6-min!G6</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>current!H6-min!H6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>current!I6-min!I6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>current!J6-min!J6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>current!C7-min!C7</f>
+        <v>-6</v>
+      </c>
+      <c r="D7">
+        <f>current!D7-min!D7</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>current!E7-min!E7</f>
+        <v>-6</v>
+      </c>
+      <c r="F7">
+        <f>current!F7-min!F7</f>
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <f>current!G7-min!G7</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>current!H7-min!H7</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>current!I7-min!I7</f>
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <f>current!J7-min!J7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f>current!C8-min!C8</f>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f>current!D8-min!D8</f>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f>current!E8-min!E8</f>
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <f>current!F8-min!F8</f>
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <f>current!G8-min!G8</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>current!H8-min!H8</f>
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <f>current!I8-min!I8</f>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>current!J8-min!J8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>current!C9-min!C9</f>
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <f>current!D9-min!D9</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>current!E9-min!E9</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>current!F9-min!F9</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>current!G9-min!G9</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>current!H9-min!H9</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>current!I9-min!I9</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>current!J9-min!J9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f>current!C10-min!C10</f>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f>current!D10-min!D10</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>current!E10-min!E10</f>
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <f>current!F10-min!F10</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>current!G10-min!G10</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>current!H10-min!H10</f>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f>current!I10-min!I10</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>current!J10-min!J10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f>current!C11-min!C11</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>current!D11-min!D11</f>
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <f>current!E11-min!E11</f>
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <f>current!F11-min!F11</f>
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <f>current!G11-min!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>current!H11-min!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>current!I11-min!I11</f>
+        <v>-1</v>
+      </c>
+      <c r="J11">
+        <f>current!J11-min!J11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f>current!C12-min!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>current!D12-min!D12</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>current!E12-min!E12</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>current!F12-min!F12</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>current!G12-min!G12</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>current!H12-min!H12</f>
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f>current!I12-min!I12</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>current!J12-min!J12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f>current!C13-min!C13</f>
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <f>current!D13-min!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>current!E13-min!E13</f>
+        <v>-2</v>
+      </c>
+      <c r="F13">
+        <f>current!F13-min!F13</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>current!G13-min!G13</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>current!H13-min!H13</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>current!I13-min!I13</f>
+        <v>-1</v>
+      </c>
+      <c r="J13">
+        <f>current!J13-min!J13</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
expanded function to work across all rows and cols
</commit_message>
<xml_diff>
--- a/staff.xlsx
+++ b/staff.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara.brumfield\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sara.brumfield\Documents\_COVID-19\GIT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
     <sheet name="min" sheetId="2" r:id="rId2"/>
+    <sheet name="diff" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
   <si>
     <t>svc</t>
   </si>
@@ -414,7 +415,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,10 +845,13 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -891,6 +895,31 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>SUM(C2:I2)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -899,6 +928,16 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="0">SUM(C3:I3)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -907,6 +946,28 @@
       <c r="B4">
         <v>2</v>
       </c>
+      <c r="C4">
+        <v>72</v>
+      </c>
+      <c r="E4">
+        <v>148</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -915,6 +976,31 @@
       <c r="B5">
         <v>2</v>
       </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -923,6 +1009,13 @@
       <c r="B6">
         <v>3</v>
       </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -931,6 +1024,22 @@
       <c r="B7">
         <v>3</v>
       </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -939,6 +1048,22 @@
       <c r="B8">
         <v>3</v>
       </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -947,6 +1072,13 @@
       <c r="B9">
         <v>3</v>
       </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -955,6 +1087,10 @@
       <c r="B10">
         <v>4</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -963,6 +1099,22 @@
       <c r="B11">
         <v>4</v>
       </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -971,6 +1123,13 @@
       <c r="B12">
         <v>4</v>
       </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -978,6 +1137,549 @@
       </c>
       <c r="B13">
         <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>current!C2-min!C2</f>
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <f>current!D2-min!D2</f>
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <f>current!E2-min!E2</f>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f>current!F2-min!F2</f>
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <f>current!G2-min!G2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <f>current!H2-min!H2</f>
+        <v>-5</v>
+      </c>
+      <c r="I2">
+        <f>current!I2-min!I2</f>
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <f>current!J2-min!J2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <f>current!C3-min!C3</f>
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <f>current!D3-min!D3</f>
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>current!E3-min!E3</f>
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <f>current!F3-min!F3</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f>current!G3-min!G3</f>
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <f>current!H3-min!H3</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f>current!I3-min!I3</f>
+        <v>-2</v>
+      </c>
+      <c r="J3">
+        <f>current!J3-min!J3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <f>current!C4-min!C4</f>
+        <v>-26</v>
+      </c>
+      <c r="D4">
+        <f>current!D4-min!D4</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>current!E4-min!E4</f>
+        <v>-4</v>
+      </c>
+      <c r="F4">
+        <f>current!F4-min!F4</f>
+        <v>-4</v>
+      </c>
+      <c r="G4">
+        <f>current!G4-min!G4</f>
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <f>current!H4-min!H4</f>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f>current!I4-min!I4</f>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <f>current!J4-min!J4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <f>current!C5-min!C5</f>
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <f>current!D5-min!D5</f>
+        <v>-6</v>
+      </c>
+      <c r="E5">
+        <f>current!E5-min!E5</f>
+        <v>16</v>
+      </c>
+      <c r="F5">
+        <f>current!F5-min!F5</f>
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <f>current!G5-min!G5</f>
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <f>current!H5-min!H5</f>
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f>current!I5-min!I5</f>
+        <v>19</v>
+      </c>
+      <c r="J5">
+        <f>current!J5-min!J5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <f>current!C6-min!C6</f>
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <f>current!D6-min!D6</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>current!E6-min!E6</f>
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <f>current!F6-min!F6</f>
+        <v>16</v>
+      </c>
+      <c r="G6">
+        <f>current!G6-min!G6</f>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f>current!H6-min!H6</f>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f>current!I6-min!I6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <f>current!J6-min!J6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <f>current!C7-min!C7</f>
+        <v>-6</v>
+      </c>
+      <c r="D7">
+        <f>current!D7-min!D7</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>current!E7-min!E7</f>
+        <v>-6</v>
+      </c>
+      <c r="F7">
+        <f>current!F7-min!F7</f>
+        <v>-1</v>
+      </c>
+      <c r="G7">
+        <f>current!G7-min!G7</f>
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <f>current!H7-min!H7</f>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f>current!I7-min!I7</f>
+        <v>-1</v>
+      </c>
+      <c r="J7">
+        <f>current!J7-min!J7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <f>current!C8-min!C8</f>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f>current!D8-min!D8</f>
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <f>current!E8-min!E8</f>
+        <v>25</v>
+      </c>
+      <c r="F8">
+        <f>current!F8-min!F8</f>
+        <v>-1</v>
+      </c>
+      <c r="G8">
+        <f>current!G8-min!G8</f>
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <f>current!H8-min!H8</f>
+        <v>9</v>
+      </c>
+      <c r="I8">
+        <f>current!I8-min!I8</f>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <f>current!J8-min!J8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <f>current!C9-min!C9</f>
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <f>current!D9-min!D9</f>
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f>current!E9-min!E9</f>
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <f>current!F9-min!F9</f>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <f>current!G9-min!G9</f>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f>current!H9-min!H9</f>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f>current!I9-min!I9</f>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <f>current!J9-min!J9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <f>current!C10-min!C10</f>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f>current!D10-min!D10</f>
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <f>current!E10-min!E10</f>
+        <v>33</v>
+      </c>
+      <c r="F10">
+        <f>current!F10-min!F10</f>
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <f>current!G10-min!G10</f>
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <f>current!H10-min!H10</f>
+        <v>10</v>
+      </c>
+      <c r="I10">
+        <f>current!I10-min!I10</f>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <f>current!J10-min!J10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <f>current!C11-min!C11</f>
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <f>current!D11-min!D11</f>
+        <v>14</v>
+      </c>
+      <c r="E11">
+        <f>current!E11-min!E11</f>
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <f>current!F11-min!F11</f>
+        <v>-1</v>
+      </c>
+      <c r="G11">
+        <f>current!G11-min!G11</f>
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <f>current!H11-min!H11</f>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f>current!I11-min!I11</f>
+        <v>-1</v>
+      </c>
+      <c r="J11">
+        <f>current!J11-min!J11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <f>current!C12-min!C12</f>
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <f>current!D12-min!D12</f>
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <f>current!E12-min!E12</f>
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>current!F12-min!F12</f>
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <f>current!G12-min!G12</f>
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <f>current!H12-min!H12</f>
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f>current!I12-min!I12</f>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <f>current!J12-min!J12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <f>current!C13-min!C13</f>
+        <v>-1</v>
+      </c>
+      <c r="D13">
+        <f>current!D13-min!D13</f>
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <f>current!E13-min!E13</f>
+        <v>-2</v>
+      </c>
+      <c r="F13">
+        <f>current!F13-min!F13</f>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <f>current!G13-min!G13</f>
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f>current!H13-min!H13</f>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f>current!I13-min!I13</f>
+        <v>-1</v>
+      </c>
+      <c r="J13">
+        <f>current!J13-min!J13</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
iter row and cols
</commit_message>
<xml_diff>
--- a/staff.xlsx
+++ b/staff.xlsx
@@ -14,7 +14,8 @@
   <sheets>
     <sheet name="current" sheetId="1" r:id="rId1"/>
     <sheet name="min" sheetId="2" r:id="rId2"/>
-    <sheet name="diff" sheetId="3" r:id="rId3"/>
+    <sheet name="pretty table" sheetId="4" r:id="rId3"/>
+    <sheet name="diff" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="47">
   <si>
     <t>svc</t>
   </si>
@@ -82,9 +83,6 @@
     <t>marine</t>
   </si>
   <si>
-    <t>emer_drivers</t>
-  </si>
-  <si>
     <t>cdl</t>
   </si>
   <si>
@@ -95,6 +93,81 @@
   </si>
   <si>
     <t>night</t>
+  </si>
+  <si>
+    <t>Service Area</t>
+  </si>
+  <si>
+    <t>Priority Level</t>
+  </si>
+  <si>
+    <t>CDLs</t>
+  </si>
+  <si>
+    <t>Non-CDL Drivers</t>
+  </si>
+  <si>
+    <t>Laborers</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Cashiers</t>
+  </si>
+  <si>
+    <t>Equipment Operators</t>
+  </si>
+  <si>
+    <t>Supervisors</t>
+  </si>
+  <si>
+    <t>Emergency Staff</t>
+  </si>
+  <si>
+    <t>Mininum Total Staff Required</t>
+  </si>
+  <si>
+    <t>Quarantine Road</t>
+  </si>
+  <si>
+    <t>Fiscal/Payroll</t>
+  </si>
+  <si>
+    <t>Routine Services</t>
+  </si>
+  <si>
+    <t>NWTS</t>
+  </si>
+  <si>
+    <t>OSS</t>
+  </si>
+  <si>
+    <t>Convenience Centers</t>
+  </si>
+  <si>
+    <t>Dirty Streets &amp; Alleys</t>
+  </si>
+  <si>
+    <t>Mechanical Street Sweeping</t>
+  </si>
+  <si>
+    <t>Special Services</t>
+  </si>
+  <si>
+    <t>Marine Operations</t>
+  </si>
+  <si>
+    <t>Night Crews</t>
+  </si>
+  <si>
+    <t>Property Management*</t>
+  </si>
+  <si>
+    <t>*Not designated a priority</t>
+  </si>
+  <si>
+    <t>emer_staff</t>
   </si>
 </sst>
 </file>
@@ -130,13 +203,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -147,6 +227,28 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K13" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:K13"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Service Area"/>
+    <tableColumn id="2" name="Priority Level"/>
+    <tableColumn id="3" name="CDLs"/>
+    <tableColumn id="4" name="Non-CDL Drivers"/>
+    <tableColumn id="5" name="Laborers"/>
+    <tableColumn id="6" name="Admin"/>
+    <tableColumn id="7" name="Cashiers"/>
+    <tableColumn id="8" name="Equipment Operators"/>
+    <tableColumn id="9" name="Supervisors"/>
+    <tableColumn id="10" name="Emergency Staff"/>
+    <tableColumn id="11" name="Mininum Total Staff Required">
+      <calculatedColumnFormula>SUM(C2:I2)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -415,7 +517,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -431,7 +533,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -452,10 +554,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -490,6 +592,7 @@
         <v>0</v>
       </c>
       <c r="K2">
+        <f>min!K2</f>
         <v>12</v>
       </c>
     </row>
@@ -525,6 +628,7 @@
         <v>0</v>
       </c>
       <c r="K3">
+        <f>min!K3</f>
         <v>9</v>
       </c>
     </row>
@@ -538,6 +642,9 @@
       <c r="C4">
         <v>46</v>
       </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
       <c r="E4">
         <f>36*4</f>
         <v>144</v>
@@ -548,6 +655,9 @@
       <c r="G4">
         <v>0</v>
       </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
       <c r="I4">
         <v>16</v>
       </c>
@@ -555,7 +665,8 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>207</v>
+        <f>min!K4</f>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -590,12 +701,13 @@
         <v>0</v>
       </c>
       <c r="K5">
+        <f>min!K5</f>
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -625,6 +737,7 @@
         <v>0</v>
       </c>
       <c r="K6">
+        <f>min!K6</f>
         <v>2</v>
       </c>
     </row>
@@ -638,19 +751,29 @@
       <c r="C7">
         <v>0</v>
       </c>
+      <c r="D7">
+        <v>5</v>
+      </c>
+      <c r="E7">
+        <v>10</v>
+      </c>
       <c r="F7">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G7">
-        <v>0</v>
+        <v>6</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
+        <f>min!K7</f>
         <v>14</v>
       </c>
     </row>
@@ -687,7 +810,8 @@
         <v>0</v>
       </c>
       <c r="K8">
-        <v>41</v>
+        <f>min!K8</f>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -700,11 +824,14 @@
       <c r="C9">
         <v>15</v>
       </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9">
         <v>0</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -719,7 +846,8 @@
         <v>0</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <f>min!K9</f>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -732,11 +860,14 @@
       <c r="C10">
         <v>10</v>
       </c>
+      <c r="D10">
+        <v>5</v>
+      </c>
       <c r="E10">
         <v>33</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -745,12 +876,13 @@
         <v>10</v>
       </c>
       <c r="I10">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10">
         <v>0</v>
       </c>
       <c r="K10">
+        <f>min!K10</f>
         <v>0</v>
       </c>
     </row>
@@ -783,7 +915,8 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>15</v>
+        <f>min!K11</f>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -800,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F12">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <v>0</v>
@@ -812,27 +945,50 @@
         <v>4</v>
       </c>
       <c r="I12">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <v>0</v>
       </c>
       <c r="K12">
+        <f>min!K12</f>
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
       <c r="J13">
         <v>0</v>
       </c>
       <c r="K13">
-        <v>12</v>
+        <f>min!K13</f>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -845,7 +1001,7 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -861,7 +1017,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -882,10 +1038,10 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="K1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1004,7 +1160,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1133,7 +1289,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -1159,10 +1315,483 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:K15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="19.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>5</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>5</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <f>SUM(C2:I2)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K13" si="0">SUM(C3:I3)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>72</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>148</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>16</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="0"/>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="83" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="K2:K13" formulaRange="1"/>
+  </ignoredErrors>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,7 +1807,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1199,7 +1828,7 @@
         <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1364,7 +1993,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1415,27 +2044,27 @@
       </c>
       <c r="D7">
         <f>current!D7-min!D7</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E7">
         <f>current!E7-min!E7</f>
-        <v>-6</v>
+        <v>4</v>
       </c>
       <c r="F7">
         <f>current!F7-min!F7</f>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G7">
         <f>current!G7-min!G7</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="H7">
         <f>current!H7-min!H7</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I7">
         <f>current!I7-min!I7</f>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J7">
         <f>current!J7-min!J7</f>
@@ -1503,7 +2132,7 @@
       </c>
       <c r="F9">
         <f>current!F9-min!F9</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G9">
         <f>current!G9-min!G9</f>
@@ -1535,7 +2164,7 @@
       </c>
       <c r="D10">
         <f>current!D10-min!D10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E10">
         <f>current!E10-min!E10</f>
@@ -1543,7 +2172,7 @@
       </c>
       <c r="F10">
         <f>current!F10-min!F10</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G10">
         <f>current!G10-min!G10</f>
@@ -1555,7 +2184,7 @@
       </c>
       <c r="I10">
         <f>current!I10-min!I10</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J10">
         <f>current!J10-min!J10</f>
@@ -1619,11 +2248,11 @@
       </c>
       <c r="E12">
         <f>current!E12-min!E12</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <f>current!F12-min!F12</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G12">
         <f>current!G12-min!G12</f>
@@ -1635,7 +2264,7 @@
       </c>
       <c r="I12">
         <f>current!I12-min!I12</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J12">
         <f>current!J12-min!J12</f>
@@ -1644,14 +2273,14 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13">
         <v>4</v>
       </c>
       <c r="C13">
         <f>current!C13-min!C13</f>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D13">
         <f>current!D13-min!D13</f>
@@ -1659,11 +2288,11 @@
       </c>
       <c r="E13">
         <f>current!E13-min!E13</f>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F13">
         <f>current!F13-min!F13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G13">
         <f>current!G13-min!G13</f>
@@ -1675,7 +2304,7 @@
       </c>
       <c r="I13">
         <f>current!I13-min!I13</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J13">
         <f>current!J13-min!J13</f>

</xml_diff>